<commit_message>
Begin portolio optimization program
</commit_message>
<xml_diff>
--- a/Computational_Investing.xlsx
+++ b/Computational_Investing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sharpe Ratio" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CAPM" sheetId="10" r:id="rId7"/>
     <sheet name="Numpy" sheetId="11" r:id="rId8"/>
     <sheet name="QSTK" sheetId="12" r:id="rId9"/>
+    <sheet name="HW1 - AssessPorfolio" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="158">
   <si>
     <t>Standard Dev of Stock's Risk</t>
   </si>
@@ -594,6 +595,39 @@
   </si>
   <si>
     <t>Accessing Data:</t>
+  </si>
+  <si>
+    <t>4 equities</t>
+  </si>
+  <si>
+    <t>Determine the best combo to get the highest Sharpe Ratio</t>
+  </si>
+  <si>
+    <t>Hold all year - 2011</t>
+  </si>
+  <si>
+    <t>Tutorial1.py</t>
+  </si>
+  <si>
+    <t>Tutorial3.py - do not use method in tuturial3 for HW1</t>
+  </si>
+  <si>
+    <t>&gt;&gt; no rebalancing</t>
+  </si>
+  <si>
+    <t>PART 1</t>
+  </si>
+  <si>
+    <t>PART 2</t>
+  </si>
+  <si>
+    <t>PART 3</t>
+  </si>
+  <si>
+    <t>use simulate() function to optimize portfolio based on allocations</t>
+  </si>
+  <si>
+    <t>created nested for loops to run different scenarios</t>
   </si>
 </sst>
 </file>
@@ -1401,6 +1435,83 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
@@ -2290,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Continue portolio optimization program
</commit_message>
<xml_diff>
--- a/Computational_Investing.xlsx
+++ b/Computational_Investing.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="187">
   <si>
     <t>Standard Dev of Stock's Risk</t>
   </si>
@@ -597,37 +597,124 @@
     <t>Accessing Data:</t>
   </si>
   <si>
-    <t>4 equities</t>
-  </si>
-  <si>
-    <t>Determine the best combo to get the highest Sharpe Ratio</t>
-  </si>
-  <si>
-    <t>Hold all year - 2011</t>
-  </si>
-  <si>
-    <t>Tutorial1.py</t>
-  </si>
-  <si>
-    <t>Tutorial3.py - do not use method in tuturial3 for HW1</t>
-  </si>
-  <si>
-    <t>&gt;&gt; no rebalancing</t>
-  </si>
-  <si>
-    <t>PART 1</t>
-  </si>
-  <si>
-    <t>PART 2</t>
-  </si>
-  <si>
-    <t>PART 3</t>
-  </si>
-  <si>
-    <t>use simulate() function to optimize portfolio based on allocations</t>
-  </si>
-  <si>
-    <t>created nested for loops to run different scenarios</t>
+    <t>1.  4 equities</t>
+  </si>
+  <si>
+    <t>2.  Determine optimal allocation that provides the best (highest) Sharpe Ratio</t>
+  </si>
+  <si>
+    <t>3.  Hold for entire year of 2011</t>
+  </si>
+  <si>
+    <t>HW - PART 1</t>
+  </si>
+  <si>
+    <t>Examples/Basic/Tutorial1.py</t>
+  </si>
+  <si>
+    <t>Examples/Basic/Tutorial3.py - do not use method in tuturial3 for HW1</t>
+  </si>
+  <si>
+    <t>&gt;&gt; no daily rebalancing</t>
+  </si>
+  <si>
+    <t>HW - PART 2</t>
+  </si>
+  <si>
+    <t>1. Write a Python function called simulate()</t>
+  </si>
+  <si>
+    <t>2. Inputs</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Symbols</t>
+  </si>
+  <si>
+    <t>Allocations</t>
+  </si>
+  <si>
+    <t>3. Outputs</t>
+  </si>
+  <si>
+    <t>Standard deviation of returns of portfolio</t>
+  </si>
+  <si>
+    <t>Average daily returns of portfolio</t>
+  </si>
+  <si>
+    <t>Cumulative return of portfolio</t>
+  </si>
+  <si>
+    <t>Figure out value of each investment every day</t>
+  </si>
+  <si>
+    <t>Call to the Function:</t>
+  </si>
+  <si>
+    <t>vol, daily_ret, sharpe, cum_ret = simulate(startdate, enddate, ['GOOG','AAPL','GLD','XOM'], [0.2,0.3,0.4,0.1])</t>
+  </si>
+  <si>
+    <t>**Check results against results on WIKI</t>
+  </si>
+  <si>
+    <t>HW - PART 3</t>
+  </si>
+  <si>
+    <t>1. Use simulate() function to build a porfolio optimizer</t>
+  </si>
+  <si>
+    <t>2. Use nested for loops that tests every legal set of allocations, i.e. &gt;&gt;</t>
+  </si>
+  <si>
+    <t>a. allocation must add up to 1.0</t>
+  </si>
+  <si>
+    <t>b. allocations increment of 0.10 only</t>
+  </si>
+  <si>
+    <t>Create a chart to plot the porfolio results (not required)</t>
+  </si>
+  <si>
+    <t>Example Output:</t>
+  </si>
+  <si>
+    <t>Start Date: January 1, 2011</t>
+  </si>
+  <si>
+    <t>End Date: December 31, 2011</t>
+  </si>
+  <si>
+    <t>Symbols: ['AAPL', 'GLD', 'GOOG', 'XOM']</t>
+  </si>
+  <si>
+    <t>Optimal Allocations: [0.4, 0.4, 0.0, 0.2]</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio: 1.02828403099</t>
+  </si>
+  <si>
+    <t>Volatility (stdev of daily returns):  0.0101467067654</t>
+  </si>
+  <si>
+    <t>Average Daily Return:  0.000657261102001</t>
+  </si>
+  <si>
+    <t>Cumulative Return:  1.16487261965</t>
+  </si>
+  <si>
+    <t>HW - PART 4</t>
+  </si>
+  <si>
+    <t>Sharpe ratio of portfolio ** (assume 252 days per year)</t>
   </si>
 </sst>
 </file>
@@ -637,7 +724,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -857,6 +944,43 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -911,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -971,6 +1095,17 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1254,7 +1389,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1437,74 +1572,250 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="G12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="49" t="s">
         <v>157</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="C25" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="45"/>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B47" s="38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B48" s="38" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="38" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue portolio optimization program hw1
</commit_message>
<xml_diff>
--- a/Computational_Investing.xlsx
+++ b/Computational_Investing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sharpe Ratio" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Question:</t>
-  </si>
-  <si>
-    <t>What is sharpe ratio for fund with avg daily return of 0.005 and stdev(daily) of 0.04; assume 250 days in the year</t>
   </si>
   <si>
     <t>S=</t>
@@ -721,6 +718,9 @@
   </si>
   <si>
     <t>Cumulative Return (Porfolio):  1.16487261965</t>
+  </si>
+  <si>
+    <t>What is sharpe ratio for fund with avg daily return of 0.005 and stdev(of daily returns) of 0.04; assume 250 days in the year</t>
   </si>
 </sst>
 </file>
@@ -1092,9 +1092,6 @@
     <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1111,6 +1108,9 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1395,8 +1395,8 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,12 +1410,12 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1430,7 +1430,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1454,14 +1454,14 @@
         <v>4</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1475,7 +1475,7 @@
         <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L11">
         <f>SQRT(250)</f>
@@ -1487,7 +1487,7 @@
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L12">
         <f>SQRT(252)</f>
@@ -1499,12 +1499,12 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1515,12 +1515,12 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1528,7 +1528,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1538,18 +1538,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
         <v>0.125</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25">
         <f>SQRT(250)</f>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26">
         <f>C25*E25</f>
@@ -1594,7 +1594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -1606,31 +1606,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1638,211 +1638,211 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="49" t="s">
-        <v>156</v>
+      <c r="B15" s="48" t="s">
+        <v>155</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="49" t="s">
-        <v>156</v>
+      <c r="B16" s="48" t="s">
+        <v>155</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="49" t="s">
-        <v>156</v>
+      <c r="B17" s="48" t="s">
+        <v>155</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="C25" s="43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="C25" s="44" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="44" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="45" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="44"/>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="45"/>
-    </row>
-    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
-        <v>179</v>
+      <c r="A37" s="46" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="48" t="s">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="37" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B42" s="38" t="s">
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="37" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B43" s="38" t="s">
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="37" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B44" s="38" t="s">
-        <v>178</v>
-      </c>
-    </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B47" s="37" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B46" s="38" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B47" s="38" t="s">
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B48" s="37" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B48" s="38" t="s">
+    <row r="49" spans="2:2" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="37" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="17" x14ac:dyDescent="0.25">
-      <c r="B49" s="38" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1868,39 +1868,39 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6">
         <v>100.1</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6">
         <v>100.05</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="9">
         <v>100</v>
@@ -1931,12 +1931,12 @@
         <v>1000</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7">
         <v>99.95</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6">
         <v>99.9</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6">
         <v>99.85</v>
@@ -1969,59 +1969,59 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2048,15 +2048,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,19 +2080,19 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2100,7 +2100,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="13"/>
     </row>
@@ -2109,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2117,7 +2117,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2125,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2133,7 +2133,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2141,7 +2141,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2149,12 +2149,12 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2197,7 +2197,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2205,17 +2205,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2223,22 +2223,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2275,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2283,7 +2283,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2291,7 +2291,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2307,7 +2307,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2335,7 +2335,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2343,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2359,97 +2359,97 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
         <v>88</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>89</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>90</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>91</v>
-      </c>
-      <c r="G8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
         <v>94</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>95</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>96</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>97</v>
-      </c>
-      <c r="G9" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
         <v>108</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
         <v>110</v>
-      </c>
-      <c r="D18" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2457,30 +2457,30 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
         <v>112</v>
-      </c>
-      <c r="D20" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B23" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2508,59 +2508,59 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" s="22"/>
       <c r="B9" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
         <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2620,13 +2620,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>142</v>
+      <c r="A1" s="39" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2639,15 +2639,15 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>129</v>
+      <c r="A6" s="36" t="s">
+        <v>128</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -2676,10 +2676,10 @@
     </row>
     <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>132</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>133</v>
       </c>
       <c r="I10">
         <v>8</v>
@@ -2692,42 +2692,42 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I13">
         <f>STDEV(I3:I11)</f>
         <v>2.7386127875258306</v>
       </c>
       <c r="J13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
         <v>135</v>
-      </c>
-      <c r="C15" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2746,18 +2746,18 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>143</v>
+      <c r="A1" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>145</v>
+      <c r="A3" s="41" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue work on allocation optimization
</commit_message>
<xml_diff>
--- a/Computational_Investing.xlsx
+++ b/Computational_Investing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="17320" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sharpe Ratio" sheetId="1" r:id="rId1"/>
@@ -1395,7 +1395,7 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -1594,14 +1594,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="7" max="14" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>